<commit_message>
Aggiunta generazione tramite gpt e aggiunto progetto alfredo senza attributi angular 19
</commit_message>
<xml_diff>
--- a/progetti-per-test/Progetto-Alfredo/confronto-pratiche-Progetto-Alfredo.xlsx
+++ b/progetti-per-test/Progetto-Alfredo/confronto-pratiche-Progetto-Alfredo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN10\Desktop\Tirocinio-aggiornato\mutanti_paper_ed_utilities\Progetto-Alfredo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN10\Desktop\Tirocinio-Aggiornato\progetti-per-test\Progetto-Alfredo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -967,7 +967,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1167,7 +1167,6 @@
         <v>46</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:D16" si="0">C11-E11-F11</f>
         <v>37</v>
       </c>
       <c r="E11" s="1">
@@ -1177,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ref="G11:G16" si="1">(E11/C11)*100</f>
+        <f t="shared" ref="G11:G16" si="0">(E11/C11)*100</f>
         <v>15.217391304347828</v>
       </c>
     </row>
@@ -1192,18 +1191,17 @@
         <v>46</v>
       </c>
       <c r="D12" s="1">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>97.826086956521735</v>
+        <v>30.434782608695656</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1217,18 +1215,17 @@
         <v>46</v>
       </c>
       <c r="D13" s="1">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="E13" s="1">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="1"/>
-        <v>23.913043478260871</v>
+        <v>21.739130434782609</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1242,18 +1239,17 @@
         <v>46</v>
       </c>
       <c r="D14" s="1">
+        <v>41</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>8.695652173913043</v>
+        <v>6.5217391304347823</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1267,18 +1263,17 @@
         <v>46</v>
       </c>
       <c r="D15" s="1">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="E15" s="1">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>23.913043478260871</v>
+        <v>21.739130434782609</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1292,18 +1287,17 @@
         <v>46</v>
       </c>
       <c r="D16" s="1">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>8.695652173913043</v>
+        <v>6.5217391304347823</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1366,15 +1360,15 @@
       </c>
       <c r="B21" s="1">
         <f>SUM(E11:E16)</f>
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1">
         <f>SUM(F11:F16)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1">
         <f>SUM(B21,C21)</f>
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>

</xml_diff>

<commit_message>
Testati con gpt tutti i progetti
</commit_message>
<xml_diff>
--- a/progetti-per-test/Progetto-Alfredo/confronto-pratiche-Progetto-Alfredo.xlsx
+++ b/progetti-per-test/Progetto-Alfredo/confronto-pratiche-Progetto-Alfredo.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Metodo di Generazione</t>
   </si>
@@ -91,13 +91,19 @@
     <t>Test con successo</t>
   </si>
   <si>
-    <t>Applicazione: angular-example-no-id - Confronto Robustezza Locatori</t>
-  </si>
-  <si>
-    <t>Totale</t>
-  </si>
-  <si>
-    <t>N\D</t>
+    <t>Generazioni mancanti</t>
+  </si>
+  <si>
+    <t>Generazioni non necessarie</t>
+  </si>
+  <si>
+    <t>Totale fallimenti</t>
+  </si>
+  <si>
+    <t>Generazioni necessarie ma errate</t>
+  </si>
+  <si>
+    <t>Applicazione: Progetto-Alfredo - Confronto Robustezza Locatori</t>
   </si>
 </sst>
 </file>
@@ -581,12 +587,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -967,7 +979,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -978,12 +990,12 @@
     <col min="4" max="4" width="24.19921875" customWidth="1"/>
     <col min="5" max="5" width="24.09765625" customWidth="1"/>
     <col min="6" max="6" width="25.69921875" customWidth="1"/>
-    <col min="7" max="7" width="25.3984375" customWidth="1"/>
+    <col min="7" max="7" width="28.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1016,20 +1028,21 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
+      <c r="C4" s="3">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G9" si="0">(E4/C4)*100</f>
+        <v>2.2727272727272729</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1039,20 +1052,21 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
+      <c r="C5" s="3">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1062,20 +1076,21 @@
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
+      <c r="C6" s="3">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>15.909090909090908</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1085,20 +1100,21 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
+      <c r="C7" s="3">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8181818181818175</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1108,20 +1124,21 @@
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
+      <c r="C8" s="3">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>15.909090909090908</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1131,20 +1148,21 @@
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
+      <c r="C9" s="3">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8181818181818175</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1176,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ref="G11:G16" si="0">(E11/C11)*100</f>
+        <f t="shared" ref="G11:G16" si="1">(E11/C11)*100</f>
         <v>15.217391304347828</v>
       </c>
     </row>
@@ -1200,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.434782608695656</v>
       </c>
     </row>
@@ -1224,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.739130434782609</v>
       </c>
     </row>
@@ -1248,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5217391304347823</v>
       </c>
     </row>
@@ -1272,7 +1290,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.739130434782609</v>
       </c>
     </row>
@@ -1296,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5217391304347823</v>
       </c>
     </row>
@@ -1331,28 +1349,43 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="1">
+        <f>SUM(E4:E9)</f>
+        <v>32</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(F4:F9)</f>
+        <v>6</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SUM(B20,C20)</f>
+        <v>38</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
@@ -1370,9 +1403,15 @@
         <f>SUM(B21,C21)</f>
         <v>59</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>